<commit_message>
Falta incorporar el fichero each_batch Pesa demasiado para subirlo a git
</commit_message>
<xml_diff>
--- a/tests/tensorflow/mnist/out/single_thread/output.xlsx
+++ b/tests/tensorflow/mnist/out/single_thread/output.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="mnist_train_papi" sheetId="1" state="visible" r:id="rId2"/>
@@ -90,13 +90,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0"/>
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
-    <numFmt numFmtId="167" formatCode="#,##0.00"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -122,6 +121,20 @@
     <font>
       <b val="true"/>
       <sz val="11"/>
+      <name val="Cambria"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
       <name val="Cambria"/>
       <family val="0"/>
       <charset val="1"/>
@@ -176,7 +189,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -201,12 +214,20 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -229,10 +250,10 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.64"/>
@@ -516,10 +537,10 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.64"/>
@@ -803,10 +824,10 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topLeft" activeCell="F36" activeCellId="0" sqref="F36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.64"/>
@@ -1089,37 +1110,38 @@
   </sheetPr>
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="3" style="6" width="18.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="3" style="1" width="18.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="18.89"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="5" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1130,22 +1152,22 @@
       <c r="B2" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="6" t="n">
+      <c r="C2" s="1" t="n">
         <v>132830362070</v>
       </c>
-      <c r="D2" s="6" t="n">
+      <c r="D2" s="1" t="n">
         <v>132828259980</v>
       </c>
-      <c r="E2" s="6" t="n">
+      <c r="E2" s="1" t="n">
         <v>132814086410</v>
       </c>
-      <c r="F2" s="6" t="n">
+      <c r="F2" s="1" t="n">
         <v>132801859154</v>
       </c>
-      <c r="G2" s="6" t="n">
+      <c r="G2" s="1" t="n">
         <v>132888970331</v>
       </c>
-      <c r="H2" s="6" t="n">
+      <c r="H2" s="2" t="n">
         <v>132832707589</v>
       </c>
     </row>
@@ -1156,22 +1178,22 @@
       <c r="B3" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="6" t="n">
+      <c r="C3" s="1" t="n">
         <v>4891139917</v>
       </c>
-      <c r="D3" s="6" t="n">
+      <c r="D3" s="1" t="n">
         <v>4890817864</v>
       </c>
-      <c r="E3" s="6" t="n">
+      <c r="E3" s="1" t="n">
         <v>4889634622</v>
       </c>
-      <c r="F3" s="6" t="n">
+      <c r="F3" s="1" t="n">
         <v>4886124317</v>
       </c>
-      <c r="G3" s="6" t="n">
+      <c r="G3" s="1" t="n">
         <v>4907140109</v>
       </c>
-      <c r="H3" s="6" t="n">
+      <c r="H3" s="2" t="n">
         <v>4892971365.8</v>
       </c>
     </row>
@@ -1182,22 +1204,22 @@
       <c r="B4" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="6" t="n">
+      <c r="C4" s="1" t="n">
         <v>48814711277</v>
       </c>
-      <c r="D4" s="6" t="n">
+      <c r="D4" s="1" t="n">
         <v>48815201214</v>
       </c>
-      <c r="E4" s="6" t="n">
+      <c r="E4" s="1" t="n">
         <v>48810558927</v>
       </c>
-      <c r="F4" s="6" t="n">
+      <c r="F4" s="1" t="n">
         <v>48809871115</v>
       </c>
-      <c r="G4" s="6" t="n">
+      <c r="G4" s="1" t="n">
         <v>48824586381</v>
       </c>
-      <c r="H4" s="6" t="n">
+      <c r="H4" s="2" t="n">
         <v>48814985782.8</v>
       </c>
     </row>
@@ -1208,22 +1230,22 @@
       <c r="B5" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="6" t="n">
+      <c r="C5" s="1" t="n">
         <v>4368069325</v>
       </c>
-      <c r="D5" s="6" t="n">
+      <c r="D5" s="1" t="n">
         <v>4368426079</v>
       </c>
-      <c r="E5" s="6" t="n">
+      <c r="E5" s="1" t="n">
         <v>4366934859</v>
       </c>
-      <c r="F5" s="6" t="n">
+      <c r="F5" s="1" t="n">
         <v>4365278614</v>
       </c>
-      <c r="G5" s="6" t="n">
+      <c r="G5" s="1" t="n">
         <v>4365119175</v>
       </c>
-      <c r="H5" s="6" t="n">
+      <c r="H5" s="2" t="n">
         <v>4366765610.4</v>
       </c>
     </row>
@@ -1234,22 +1256,22 @@
       <c r="B6" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="6" t="n">
+      <c r="C6" s="1" t="n">
         <v>239661702</v>
       </c>
-      <c r="D6" s="6" t="n">
+      <c r="D6" s="1" t="n">
         <v>239661275</v>
       </c>
-      <c r="E6" s="6" t="n">
+      <c r="E6" s="1" t="n">
         <v>239661279</v>
       </c>
-      <c r="F6" s="6" t="n">
+      <c r="F6" s="1" t="n">
         <v>239661351</v>
       </c>
-      <c r="G6" s="6" t="n">
+      <c r="G6" s="1" t="n">
         <v>239661162</v>
       </c>
-      <c r="H6" s="6" t="n">
+      <c r="H6" s="2" t="n">
         <v>239661353.8</v>
       </c>
     </row>
@@ -1260,22 +1282,22 @@
       <c r="B7" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="6" t="n">
+      <c r="C7" s="1" t="n">
         <v>152115060</v>
       </c>
-      <c r="D7" s="6" t="n">
+      <c r="D7" s="1" t="n">
         <v>152115060</v>
       </c>
-      <c r="E7" s="6" t="n">
+      <c r="E7" s="1" t="n">
         <v>152115060</v>
       </c>
-      <c r="F7" s="6" t="n">
+      <c r="F7" s="1" t="n">
         <v>152115060</v>
       </c>
-      <c r="G7" s="6" t="n">
+      <c r="G7" s="1" t="n">
         <v>152115060</v>
       </c>
-      <c r="H7" s="6" t="n">
+      <c r="H7" s="2" t="n">
         <v>152115060</v>
       </c>
     </row>
@@ -1286,22 +1308,22 @@
       <c r="B8" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="6" t="n">
+      <c r="C8" s="1" t="n">
         <v>15150000</v>
       </c>
-      <c r="D8" s="6" t="n">
+      <c r="D8" s="1" t="n">
         <v>15150000</v>
       </c>
-      <c r="E8" s="6" t="n">
+      <c r="E8" s="1" t="n">
         <v>15150000</v>
       </c>
-      <c r="F8" s="6" t="n">
+      <c r="F8" s="1" t="n">
         <v>15150000</v>
       </c>
-      <c r="G8" s="6" t="n">
+      <c r="G8" s="1" t="n">
         <v>15150000</v>
       </c>
-      <c r="H8" s="6" t="n">
+      <c r="H8" s="2" t="n">
         <v>15150000</v>
       </c>
     </row>
@@ -1312,22 +1334,22 @@
       <c r="B9" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="6" t="n">
+      <c r="C9" s="1" t="n">
         <v>3345001</v>
       </c>
-      <c r="D9" s="6" t="n">
+      <c r="D9" s="1" t="n">
         <v>3345001</v>
       </c>
-      <c r="E9" s="6" t="n">
+      <c r="E9" s="1" t="n">
         <v>3345001</v>
       </c>
-      <c r="F9" s="6" t="n">
+      <c r="F9" s="1" t="n">
         <v>3345001</v>
       </c>
-      <c r="G9" s="6" t="n">
+      <c r="G9" s="1" t="n">
         <v>3345001</v>
       </c>
-      <c r="H9" s="6" t="n">
+      <c r="H9" s="2" t="n">
         <v>3345001</v>
       </c>
     </row>
@@ -1338,22 +1360,22 @@
       <c r="B10" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="6" t="n">
+      <c r="C10" s="1" t="n">
         <v>120849165006</v>
       </c>
-      <c r="D10" s="6" t="n">
+      <c r="D10" s="1" t="n">
         <v>120849165006</v>
       </c>
-      <c r="E10" s="6" t="n">
+      <c r="E10" s="1" t="n">
         <v>120849165006</v>
       </c>
-      <c r="F10" s="6" t="n">
+      <c r="F10" s="1" t="n">
         <v>120849165006</v>
       </c>
-      <c r="G10" s="6" t="n">
+      <c r="G10" s="1" t="n">
         <v>120849165006</v>
       </c>
-      <c r="H10" s="6" t="n">
+      <c r="H10" s="2" t="n">
         <v>120849165006</v>
       </c>
     </row>
@@ -1375,206 +1397,212 @@
   </sheetPr>
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="2" width="17.78"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="6"/>
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="8" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="n">
+      <c r="A2" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="9" t="n">
         <v>192683095523.6</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="9" t="n">
         <v>192924787668.6</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="9" t="n">
         <v>192628247322.6</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="9" t="n">
         <v>132832707589</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="n">
+      <c r="A3" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="9" t="n">
         <v>16523790876.2</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="9" t="n">
         <v>16563398880.6</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="9" t="n">
         <v>16511912796.8</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3" s="9" t="n">
         <v>4892971365.8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="n">
+      <c r="A4" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="9" t="n">
         <v>66953468535.8</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="9" t="n">
         <v>67024252859.2</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="9" t="n">
         <v>66963761027.4</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4" s="9" t="n">
         <v>48814985782.8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="n">
+      <c r="A5" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="9" t="n">
         <v>15452556254</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="9" t="n">
         <v>15535692196.8</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="9" t="n">
         <v>15499554514</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5" s="9" t="n">
         <v>4366765610.4</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="n">
+      <c r="A6" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="9" t="n">
         <v>247234583.4</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="9" t="n">
         <v>247281169.6</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="9" t="n">
         <v>247235346.6</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6" s="9" t="n">
         <v>239661353.8</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="n">
+      <c r="A7" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="9" t="n">
         <v>154688753</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="9" t="n">
         <v>154688753</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7" s="9" t="n">
         <v>154688693</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="F7" s="9" t="n">
         <v>152115060</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="n">
+      <c r="A8" s="7" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="0" t="n">
-        <v>15056280</v>
-      </c>
-      <c r="D8" s="0" t="n">
-        <v>15056280</v>
-      </c>
-      <c r="E8" s="0" t="n">
-        <v>15056280</v>
-      </c>
-      <c r="F8" s="0" t="n">
+      <c r="C8" s="9" t="n">
+        <v>15056280</v>
+      </c>
+      <c r="D8" s="9" t="n">
+        <v>15056280</v>
+      </c>
+      <c r="E8" s="9" t="n">
+        <v>15056280</v>
+      </c>
+      <c r="F8" s="9" t="n">
         <v>15150000</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="n">
+      <c r="A9" s="7" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="0" t="n">
-        <v>3403140</v>
-      </c>
-      <c r="D9" s="0" t="n">
-        <v>3403140</v>
-      </c>
-      <c r="E9" s="0" t="n">
-        <v>3403140</v>
-      </c>
-      <c r="F9" s="0" t="n">
+      <c r="C9" s="9" t="n">
+        <v>3403140</v>
+      </c>
+      <c r="D9" s="9" t="n">
+        <v>3403140</v>
+      </c>
+      <c r="E9" s="9" t="n">
+        <v>3403140</v>
+      </c>
+      <c r="F9" s="9" t="n">
         <v>3345001</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="n">
+      <c r="A10" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="0" t="n">
-        <v>122693346870</v>
-      </c>
-      <c r="D10" s="0" t="n">
-        <v>122693346870</v>
-      </c>
-      <c r="E10" s="0" t="n">
-        <v>122693346870</v>
-      </c>
-      <c r="F10" s="0" t="n">
+      <c r="C10" s="9" t="n">
+        <v>122693346870</v>
+      </c>
+      <c r="D10" s="9" t="n">
+        <v>122693346870</v>
+      </c>
+      <c r="E10" s="9" t="n">
+        <v>122693346870</v>
+      </c>
+      <c r="F10" s="9" t="n">
         <v>120849165006</v>
       </c>
     </row>

</xml_diff>